<commit_message>
Implemented Excell Table wrapper
</commit_message>
<xml_diff>
--- a/test/src/org/tms/tds/excel/xls/sample1.xlsx
+++ b/test/src/org/tms/tds/excel/xls/sample1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -21,12 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t xml:space="preserve"> A</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> C</t>
-  </si>
-  <si>
     <t>Blue Row</t>
   </si>
   <si>
@@ -52,6 +46,12 @@
   </si>
   <si>
     <t>Cyan</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -424,45 +424,46 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>13000</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -470,27 +471,28 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>-12</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>17.649999999999999</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>

</xml_diff>